<commit_message>
Updated readme.md and locustfile.py
Updated README.md with detailed instructions on how to run the project
Added screenshots
Updated locustfile.py to automatically set the host
</commit_message>
<xml_diff>
--- a/Yearly Project Management Plan.xlsx
+++ b/Yearly Project Management Plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdim/Desktop/Work2020/UdacityAzureDevOps/Udacity-AzureDevOps-BuildingA_CI-CD_Pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2D95AD-4F0F-6342-B3B3-0C79A96B77CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF58F4-F4D0-4C4C-A019-4E2036FB137E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="22040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="840" windowWidth="38400" windowHeight="20720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t>Week</t>
   </si>
@@ -228,6 +229,9 @@
   <si>
     <t>PROJECT: Build a CI/CD pipeline</t>
   </si>
+  <si>
+    <t>&lt;component&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -414,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -435,59 +439,32 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -496,9 +473,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,7 +736,7 @@
   </sheetPr>
   <dimension ref="A1:AB1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="123" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -735,15 +751,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15"/>
@@ -787,21 +803,21 @@
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>44105</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="19"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -824,15 +840,15 @@
       <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19">
+      <c r="A4" s="40"/>
+      <c r="B4" s="18">
         <v>44112</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="23" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="2"/>
@@ -857,17 +873,17 @@
       <c r="AB4" s="2"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19">
+      <c r="A5" s="40"/>
+      <c r="B5" s="18">
         <v>44119</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="24"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="21"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -890,15 +906,15 @@
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19">
+      <c r="A6" s="40"/>
+      <c r="B6" s="18">
         <v>44126</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="23" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="2"/>
@@ -923,17 +939,17 @@
       <c r="AB6" s="2"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19">
+      <c r="A7" s="40"/>
+      <c r="B7" s="18">
         <v>44133</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="24"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="21"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -956,15 +972,15 @@
       <c r="AB7" s="2"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19">
+      <c r="A8" s="40"/>
+      <c r="B8" s="18">
         <v>44140</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="23" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="2"/>
@@ -989,19 +1005,19 @@
       <c r="AB8" s="2"/>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19">
+      <c r="A9" s="40"/>
+      <c r="B9" s="18">
         <v>44147</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="24"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="21"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1024,15 +1040,15 @@
       <c r="AB9" s="2"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19">
+      <c r="A10" s="40"/>
+      <c r="B10" s="18">
         <v>44154</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="23" t="s">
+      <c r="C10" s="39"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="2"/>
@@ -1057,17 +1073,17 @@
       <c r="AB10" s="2"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19">
+      <c r="A11" s="40"/>
+      <c r="B11" s="18">
         <v>44161</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="21" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="21"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1090,15 +1106,15 @@
       <c r="AB11" s="2"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19">
+      <c r="A12" s="40"/>
+      <c r="B12" s="18">
         <v>44168</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="23" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I12" s="2"/>
@@ -1123,17 +1139,17 @@
       <c r="AB12" s="2"/>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19">
+      <c r="A13" s="40"/>
+      <c r="B13" s="18">
         <v>44175</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="21" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1156,15 +1172,15 @@
       <c r="AB13" s="2"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19">
+      <c r="A14" s="40"/>
+      <c r="B14" s="18">
         <v>44182</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="23" t="s">
+      <c r="C14" s="39"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="2"/>
@@ -1189,17 +1205,17 @@
       <c r="AB14" s="2"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19">
+      <c r="A15" s="40"/>
+      <c r="B15" s="18">
         <v>44189</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="21" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="22"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="19"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1222,15 +1238,15 @@
       <c r="AB15" s="2"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19">
+      <c r="A16" s="40"/>
+      <c r="B16" s="18">
         <v>44196</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="23" t="s">
+      <c r="C16" s="39"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I16" s="2"/>
@@ -1255,21 +1271,21 @@
       <c r="AB16" s="2"/>
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <v>44203</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1292,15 +1308,15 @@
       <c r="AB17" s="2"/>
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="29"/>
-      <c r="B18" s="19">
+      <c r="A18" s="41"/>
+      <c r="B18" s="18">
         <v>44210</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="23" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I18" s="2"/>
@@ -1325,17 +1341,17 @@
       <c r="AB18" s="2"/>
     </row>
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="29"/>
-      <c r="B19" s="19">
+      <c r="A19" s="41"/>
+      <c r="B19" s="18">
         <v>44217</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="37"/>
+      <c r="D19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1358,15 +1374,15 @@
       <c r="AB19" s="2"/>
     </row>
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="29"/>
-      <c r="B20" s="19">
+      <c r="A20" s="41"/>
+      <c r="B20" s="18">
         <v>44224</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="23" t="s">
+      <c r="C20" s="37"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I20" s="2"/>
@@ -1391,17 +1407,17 @@
       <c r="AB20" s="2"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="29"/>
-      <c r="B21" s="19">
+      <c r="A21" s="41"/>
+      <c r="B21" s="18">
         <v>44231</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="21" t="s">
+      <c r="C21" s="37"/>
+      <c r="D21" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1424,15 +1440,15 @@
       <c r="AB21" s="2"/>
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="29"/>
-      <c r="B22" s="19">
+      <c r="A22" s="41"/>
+      <c r="B22" s="18">
         <v>44238</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="23" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I22" s="2"/>
@@ -1457,17 +1473,17 @@
       <c r="AB22" s="2"/>
     </row>
     <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="29"/>
-      <c r="B23" s="19">
+      <c r="A23" s="41"/>
+      <c r="B23" s="18">
         <v>44245</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="21" t="s">
+      <c r="C23" s="37"/>
+      <c r="D23" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1490,15 +1506,15 @@
       <c r="AB23" s="2"/>
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="29"/>
-      <c r="B24" s="19">
+      <c r="A24" s="41"/>
+      <c r="B24" s="18">
         <v>44252</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="23" t="s">
+      <c r="C24" s="37"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I24" s="2"/>
@@ -1523,17 +1539,17 @@
       <c r="AB24" s="2"/>
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="29"/>
-      <c r="B25" s="19">
+      <c r="A25" s="41"/>
+      <c r="B25" s="18">
         <v>44259</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="21" t="s">
+      <c r="C25" s="37"/>
+      <c r="D25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1556,15 +1572,15 @@
       <c r="AB25" s="2"/>
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="29"/>
-      <c r="B26" s="19">
+      <c r="A26" s="41"/>
+      <c r="B26" s="18">
         <v>44266</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="23" t="s">
+      <c r="C26" s="37"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="2"/>
@@ -1589,17 +1605,17 @@
       <c r="AB26" s="2"/>
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="29"/>
-      <c r="B27" s="19">
+      <c r="A27" s="41"/>
+      <c r="B27" s="18">
         <v>44273</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="21" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="22"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="19"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1622,15 +1638,15 @@
       <c r="AB27" s="2"/>
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="29"/>
-      <c r="B28" s="19">
+      <c r="A28" s="41"/>
+      <c r="B28" s="18">
         <v>44280</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="23" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I28" s="2"/>
@@ -1655,21 +1671,21 @@
       <c r="AB28" s="2"/>
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="18">
         <v>44287</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1692,15 +1708,15 @@
       <c r="AB29" s="2"/>
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="29"/>
-      <c r="B30" s="19">
+      <c r="A30" s="41"/>
+      <c r="B30" s="18">
         <v>44294</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="23" t="s">
+      <c r="C30" s="35"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I30" s="2"/>
@@ -1725,17 +1741,17 @@
       <c r="AB30" s="2"/>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="29"/>
-      <c r="B31" s="19">
+      <c r="A31" s="41"/>
+      <c r="B31" s="18">
         <v>44301</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="21" t="s">
+      <c r="C31" s="35"/>
+      <c r="D31" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="24"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="21"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1758,15 +1774,15 @@
       <c r="AB31" s="2"/>
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="29"/>
-      <c r="B32" s="19">
+      <c r="A32" s="41"/>
+      <c r="B32" s="18">
         <v>44308</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="23" t="s">
+      <c r="C32" s="35"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I32" s="2"/>
@@ -1791,17 +1807,17 @@
       <c r="AB32" s="2"/>
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="29"/>
-      <c r="B33" s="19">
+      <c r="A33" s="41"/>
+      <c r="B33" s="18">
         <v>44315</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="33" t="s">
+      <c r="C33" s="35"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="24"/>
+      <c r="G33" s="21"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
@@ -1824,15 +1840,15 @@
       <c r="AB33" s="2"/>
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="29"/>
-      <c r="B34" s="19">
+      <c r="A34" s="41"/>
+      <c r="B34" s="18">
         <v>44322</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="23" t="s">
+      <c r="C34" s="35"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I34" s="2"/>
@@ -1857,19 +1873,19 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="29"/>
-      <c r="B35" s="19">
+      <c r="A35" s="41"/>
+      <c r="B35" s="18">
         <v>44329</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="35" t="s">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="24"/>
+      <c r="G35" s="21"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -1892,15 +1908,15 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="29"/>
-      <c r="B36" s="19">
+      <c r="A36" s="41"/>
+      <c r="B36" s="18">
         <v>44336</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="23" t="s">
+      <c r="C36" s="25"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I36" s="2"/>
@@ -1925,17 +1941,17 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="29"/>
-      <c r="B37" s="19">
+      <c r="A37" s="41"/>
+      <c r="B37" s="18">
         <v>44343</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="33" t="s">
+      <c r="C37" s="25"/>
+      <c r="D37" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="24"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="21"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -1958,15 +1974,15 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="29"/>
-      <c r="B38" s="19">
+      <c r="A38" s="41"/>
+      <c r="B38" s="18">
         <v>44350</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="23" t="s">
+      <c r="C38" s="25"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I38" s="2"/>
@@ -1991,17 +2007,17 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="29"/>
-      <c r="B39" s="19">
+      <c r="A39" s="41"/>
+      <c r="B39" s="18">
         <v>44357</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="33" t="s">
+      <c r="C39" s="25"/>
+      <c r="D39" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="33"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="22"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="19"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2024,15 +2040,15 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="29"/>
-      <c r="B40" s="19">
+      <c r="A40" s="41"/>
+      <c r="B40" s="18">
         <v>44364</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="23" t="s">
+      <c r="C40" s="25"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I40" s="2"/>
@@ -2057,15 +2073,15 @@
       <c r="AB40" s="2"/>
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="29"/>
-      <c r="B41" s="19">
+      <c r="A41" s="41"/>
+      <c r="B41" s="18">
         <v>44371</v>
       </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -2088,21 +2104,21 @@
       <c r="AB41" s="2"/>
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="18">
         <v>44378</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="24"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="21"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -2125,15 +2141,15 @@
       <c r="AB42" s="2"/>
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="29"/>
-      <c r="B43" s="19">
+      <c r="A43" s="41"/>
+      <c r="B43" s="18">
         <v>44385</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="23" t="s">
+      <c r="C43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I43" s="2"/>
@@ -2158,17 +2174,17 @@
       <c r="AB43" s="2"/>
     </row>
     <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="29"/>
-      <c r="B44" s="19">
+      <c r="A44" s="41"/>
+      <c r="B44" s="18">
         <v>44392</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="35" t="s">
+      <c r="C44" s="27"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="21"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
@@ -2191,15 +2207,15 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="29"/>
-      <c r="B45" s="19">
+      <c r="A45" s="41"/>
+      <c r="B45" s="18">
         <v>44399</v>
       </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="23" t="s">
+      <c r="C45" s="27"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I45" s="2"/>
@@ -2224,17 +2240,17 @@
       <c r="AB45" s="2"/>
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="29"/>
-      <c r="B46" s="19">
+      <c r="A46" s="41"/>
+      <c r="B46" s="18">
         <v>44406</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="33" t="s">
+      <c r="C46" s="27"/>
+      <c r="D46" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="24"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="21"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -2257,15 +2273,15 @@
       <c r="AB46" s="2"/>
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="29"/>
-      <c r="B47" s="19">
+      <c r="A47" s="41"/>
+      <c r="B47" s="18">
         <v>44413</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="23" t="s">
+      <c r="C47" s="27"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I47" s="2"/>
@@ -2290,19 +2306,19 @@
       <c r="AB47" s="2"/>
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="29"/>
-      <c r="B48" s="19">
+      <c r="A48" s="41"/>
+      <c r="B48" s="18">
         <v>44420</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="39" t="s">
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="24"/>
+      <c r="G48" s="21"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -2325,15 +2341,15 @@
       <c r="AB48" s="2"/>
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="29"/>
-      <c r="B49" s="19">
+      <c r="A49" s="41"/>
+      <c r="B49" s="18">
         <v>44427</v>
       </c>
-      <c r="C49" s="36"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="23" t="s">
+      <c r="C49" s="25"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I49" s="2"/>
@@ -2358,17 +2374,17 @@
       <c r="AB49" s="2"/>
     </row>
     <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="29"/>
-      <c r="B50" s="19">
+      <c r="A50" s="41"/>
+      <c r="B50" s="18">
         <v>44434</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="39" t="s">
+      <c r="C50" s="25"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="G50" s="24"/>
+      <c r="G50" s="21"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -2391,15 +2407,15 @@
       <c r="AB50" s="2"/>
     </row>
     <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="29"/>
-      <c r="B51" s="19">
+      <c r="A51" s="41"/>
+      <c r="B51" s="18">
         <v>44441</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="23" t="s">
+      <c r="C51" s="25"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I51" s="2"/>
@@ -2424,17 +2440,17 @@
       <c r="AB51" s="2"/>
     </row>
     <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="29"/>
-      <c r="B52" s="19">
+      <c r="A52" s="41"/>
+      <c r="B52" s="18">
         <v>44448</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="39" t="s">
+      <c r="C52" s="25"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="G52" s="24"/>
+      <c r="G52" s="21"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -2457,15 +2473,15 @@
       <c r="AB52" s="2"/>
     </row>
     <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="29"/>
-      <c r="B53" s="19">
+      <c r="A53" s="41"/>
+      <c r="B53" s="18">
         <v>44455</v>
       </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="23" t="s">
+      <c r="C53" s="25"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I53" s="2"/>
@@ -2490,19 +2506,19 @@
       <c r="AB53" s="2"/>
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="29"/>
-      <c r="B54" s="19">
+      <c r="A54" s="41"/>
+      <c r="B54" s="18">
         <v>44462</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="26"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="22"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -30206,6 +30222,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="A17:A28"/>
+    <mergeCell ref="A29:A41"/>
+    <mergeCell ref="A42:A54"/>
+    <mergeCell ref="D9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C16"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="D5:F6"/>
+    <mergeCell ref="D7:F8"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="D31:E32"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="C35:C41"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="D37:E38"/>
+    <mergeCell ref="D39:E40"/>
     <mergeCell ref="C48:C53"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C42:C47"/>
@@ -30215,15 +30253,6 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F50:F51"/>
     <mergeCell ref="F52:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="D31:E32"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="C35:C41"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D37:E38"/>
-    <mergeCell ref="D39:E40"/>
     <mergeCell ref="D19:E20"/>
     <mergeCell ref="D17:E18"/>
     <mergeCell ref="C17:C28"/>
@@ -30231,20 +30260,446 @@
     <mergeCell ref="D23:E24"/>
     <mergeCell ref="D25:E26"/>
     <mergeCell ref="D27:E28"/>
-    <mergeCell ref="D9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C16"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="D5:F6"/>
-    <mergeCell ref="D7:F8"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="A17:A28"/>
-    <mergeCell ref="A29:A41"/>
-    <mergeCell ref="A42:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE67B086-FAF6-B042-B632-922556E0DBB5}">
+  <dimension ref="A1:Z14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+    </row>
+    <row r="2" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="46">
+        <v>44105</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+    </row>
+    <row r="3" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="46">
+        <v>44112</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+    </row>
+    <row r="4" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="46">
+        <v>44119</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+    </row>
+    <row r="5" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="46">
+        <v>44126</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+    </row>
+    <row r="6" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="46">
+        <v>44133</v>
+      </c>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+    </row>
+    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="46">
+        <v>44140</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+    </row>
+    <row r="8" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="46">
+        <v>44147</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+    </row>
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="46">
+        <v>44154</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="48"/>
+    </row>
+    <row r="10" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="46">
+        <v>44161</v>
+      </c>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48"/>
+    </row>
+    <row r="11" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="46">
+        <v>44168</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+    </row>
+    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="46">
+        <v>44175</v>
+      </c>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+    </row>
+    <row r="13" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="46">
+        <v>44182</v>
+      </c>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+    </row>
+    <row r="14" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="49"/>
+      <c r="B14" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>